<commit_message>
LDES example working to be filled up with actual data
Co-Authored-By: SamBaldwinDOE <45411063+SamBaldwinDOE@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/technology/ldes/datastructure.xlsx
+++ b/src/technology/ldes/datastructure.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tghosh/Library/CloudStorage/OneDrive-NREL/work_NREL/tyche/src/technology/ldes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nrel-my.sharepoint.com/personal/tghosh_nrel_gov/Documents/work_NREL/tyche/src/technology/ldes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E293F4-5012-9A4C-8540-B99822086119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{F6E293F4-5012-9A4C-8540-B99822086119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48C49E3F-3D33-434E-A013-04C33BD792E3}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="2460" windowWidth="34560" windowHeight="19880" xr2:uid="{83FFFD7F-A1DD-4846-8FB6-71F940EEADB4}"/>
+    <workbookView xWindow="42340" yWindow="500" windowWidth="34560" windowHeight="19880" xr2:uid="{83FFFD7F-A1DD-4846-8FB6-71F940EEADB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
   <si>
     <t>Rectifier</t>
   </si>
@@ -92,9 +92,6 @@
     <t>AC Electricity</t>
   </si>
   <si>
-    <t>Conversion Factor</t>
-  </si>
-  <si>
     <t>Lifetime</t>
   </si>
   <si>
@@ -105,13 +102,28 @@
   </si>
   <si>
     <t>Technology model Python file</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>Conversion Factor, Efficiency</t>
+  </si>
+  <si>
+    <t>Efficiency/loss factor</t>
+  </si>
+  <si>
+    <t>Conversion Factor,Efficiency</t>
+  </si>
+  <si>
+    <t>Scale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -134,8 +146,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,6 +231,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -242,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -260,6 +285,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -287,8 +313,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>365579</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2981174</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>16256</xdr:rowOff>
     </xdr:to>
@@ -625,17 +651,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B88606BA-60E8-0342-A934-504CC4F264D5}">
   <dimension ref="A8:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="53.33203125" customWidth="1"/>
+    <col min="4" max="4" width="63.6640625" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
     <col min="6" max="6" width="24.33203125" customWidth="1"/>
     <col min="7" max="7" width="20.33203125" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
     <col min="9" max="9" width="19.33203125" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" customWidth="1"/>
   </cols>
@@ -757,9 +786,7 @@
       <c r="H12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="I12" s="12"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -767,36 +794,30 @@
         <v>14</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>18</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D13" s="13"/>
       <c r="E13" s="13" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>18</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G13" s="17"/>
       <c r="H13" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>18</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="13"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>0</v>
@@ -824,24 +845,29 @@
       </c>
       <c r="J14" s="4" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="14"/>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="15"/>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="16"/>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>